<commit_message>
update data citing and optimization function
</commit_message>
<xml_diff>
--- a/Table1_for_code.xlsx
+++ b/Table1_for_code.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox/Modeling Project/Data_modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DoerLBH/Dropbox/git/TengLab_Ebola_GUI_SL/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUI" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Month</t>
+  </si>
+  <si>
+    <t>Infectious</t>
   </si>
 </sst>
 </file>
@@ -448,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="A1:E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -467,10 +470,13 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,10 +487,14 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <f>B2-C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -495,10 +505,14 @@
         <v>83</v>
       </c>
       <c r="D3">
+        <f t="shared" ref="D3:D18" si="0">B3-C3</f>
+        <v>44</v>
+      </c>
+      <c r="E3">
         <v>65.349999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,10 +523,14 @@
         <v>149</v>
       </c>
       <c r="D4">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="E4">
         <v>65.930000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -523,10 +541,14 @@
         <v>208</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="E5">
         <v>63.41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -537,10 +559,14 @@
         <v>303</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="E6">
         <v>73.37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -551,10 +577,14 @@
         <v>358</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="E7">
         <v>73.81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -565,10 +595,14 @@
         <v>494</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>277</v>
+      </c>
+      <c r="E8">
         <v>64.069999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -579,10 +613,14 @@
         <v>739</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="E9">
         <v>61.63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -593,10 +631,14 @@
         <v>1018</v>
       </c>
       <c r="D10">
+        <f t="shared" si="0"/>
+        <v>649</v>
+      </c>
+      <c r="E10">
         <v>61.07</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -607,10 +649,14 @@
         <v>1327</v>
       </c>
       <c r="D11">
+        <f t="shared" si="0"/>
+        <v>837</v>
+      </c>
+      <c r="E11">
         <v>61.32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -621,10 +667,14 @@
         <v>1708</v>
       </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>999</v>
+      </c>
+      <c r="E12">
         <v>63.1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -635,10 +685,14 @@
         <v>1944</v>
       </c>
       <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1031</v>
+      </c>
+      <c r="E13">
         <v>65.34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -649,10 +703,14 @@
         <v>2129</v>
       </c>
       <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1090</v>
+      </c>
+      <c r="E14">
         <v>66.14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -663,10 +721,14 @@
         <v>2314</v>
       </c>
       <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1178</v>
+      </c>
+      <c r="E15">
         <v>66.27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -677,10 +739,14 @@
         <v>2377</v>
       </c>
       <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1207</v>
+      </c>
+      <c r="E16">
         <v>66.319999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -691,10 +757,14 @@
         <v>2429</v>
       </c>
       <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1223</v>
+      </c>
+      <c r="E17">
         <v>66.510000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -705,6 +775,10 @@
         <v>2482</v>
       </c>
       <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1247</v>
+      </c>
+      <c r="E18">
         <v>66.56</v>
       </c>
     </row>
@@ -715,15 +789,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -734,10 +808,13 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -748,10 +825,14 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <f>B2-C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -762,10 +843,14 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" ref="D3:D18" si="0">B3-C3</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -776,10 +861,14 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -790,10 +879,14 @@
         <v>6</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="E5">
         <v>7.59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -804,10 +897,14 @@
         <v>99</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="E6">
         <v>41.42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -818,10 +915,14 @@
         <v>273</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>373</v>
+      </c>
+      <c r="E7">
         <v>42.26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -832,10 +933,14 @@
         <v>476</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>740</v>
+      </c>
+      <c r="E8">
         <v>39.14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -846,10 +951,14 @@
         <v>623</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1814</v>
+      </c>
+      <c r="E9">
         <v>25.56</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -860,10 +969,14 @@
         <v>1510</v>
       </c>
       <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3828</v>
+      </c>
+      <c r="E10">
         <v>28.29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -874,10 +987,14 @@
         <v>1583</v>
       </c>
       <c r="D11">
+        <f t="shared" si="0"/>
+        <v>5729</v>
+      </c>
+      <c r="E11">
         <v>21.65</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -888,10 +1005,14 @@
         <v>2758</v>
       </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6688</v>
+      </c>
+      <c r="E12">
         <v>29.2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -902,10 +1023,14 @@
         <v>3276</v>
       </c>
       <c r="D13">
+        <f t="shared" si="0"/>
+        <v>7464</v>
+      </c>
+      <c r="E13">
         <v>30.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -916,10 +1041,14 @@
         <v>3546</v>
       </c>
       <c r="D14">
+        <f t="shared" si="0"/>
+        <v>7920</v>
+      </c>
+      <c r="E14">
         <v>30.93</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -930,10 +1059,14 @@
         <v>3799</v>
       </c>
       <c r="D15">
+        <f t="shared" si="0"/>
+        <v>8175</v>
+      </c>
+      <c r="E15">
         <v>31.73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -944,10 +1077,14 @@
         <v>3899</v>
       </c>
       <c r="D16">
+        <f t="shared" si="0"/>
+        <v>8472</v>
+      </c>
+      <c r="E16">
         <v>31.52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -958,10 +1095,14 @@
         <v>3912</v>
       </c>
       <c r="D17">
+        <f t="shared" si="0"/>
+        <v>8915</v>
+      </c>
+      <c r="E17">
         <v>30.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -972,6 +1113,10 @@
         <v>3932</v>
       </c>
       <c r="D18">
+        <f t="shared" si="0"/>
+        <v>9187</v>
+      </c>
+      <c r="E18">
         <v>29.97</v>
       </c>
     </row>

</xml_diff>